<commit_message>
added final output for survey data
</commit_message>
<xml_diff>
--- a/survey/anondata2.xlsx
+++ b/survey/anondata2.xlsx
@@ -15,9 +15,6 @@
     <sheet name="Survey Responses" sheetId="1" r:id="rId1"/>
     <sheet name="Topic Subjects" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -141,13 +138,13 @@
     <t>Increase reporting of adult immunizations to ALERT IIS</t>
   </si>
   <si>
-    <t>Education strategies to address vaccine-hesitancy</t>
-  </si>
-  <si>
     <t>Allow private child care facilities to exclude those with non-medical exemptions</t>
   </si>
   <si>
     <t>Encouraging teens to self-refer for immunizations</t>
+  </si>
+  <si>
+    <t>Education strategies to address vaccine hesitancy</t>
   </si>
 </sst>
 </file>
@@ -203,19 +200,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1176,7 +1160,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1205,7 +1189,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
@@ -1213,7 +1197,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
@@ -1221,7 +1205,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">

</xml_diff>